<commit_message>
Results images with masks.
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Results!$A$1:$L$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Results!$A$1:$L$40</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="156">
   <si>
     <t>Classifier</t>
   </si>
@@ -490,13 +490,25 @@
   </si>
   <si>
     <t>01m00.105s</t>
+  </si>
+  <si>
+    <t>00m20.932s</t>
+  </si>
+  <si>
+    <t>00m17.985s</t>
+  </si>
+  <si>
+    <t>00m37.934s</t>
+  </si>
+  <si>
+    <t>03m33.083s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +538,12 @@
       <color theme="2" tint="-0.749992370372631"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -666,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -710,25 +728,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1056,6 +1072,50 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1091,36 +1151,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1135,24 +1165,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A2:L31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="0" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
-  <autoFilter ref="A2:L31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A2:L32" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A2:L32"/>
   <sortState ref="A2:L30">
     <sortCondition descending="1" ref="J1:J36"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="Feature_x000a_detector" dataDxfId="12"/>
-    <tableColumn id="2" name="Feature_x000a_descriptor" dataDxfId="11"/>
-    <tableColumn id="3" name="Feature_x000a_matcher" dataDxfId="10"/>
-    <tableColumn id="4" name="Classifier" dataDxfId="9"/>
-    <tableColumn id="5" name="Vocabulary build time_x000a_(1000 word size - 177 images)" dataDxfId="8"/>
-    <tableColumn id="6" name="Training samples build time_x000a_(177 images)" dataDxfId="7"/>
-    <tableColumn id="7" name="Training samples retrieved_x000a_(from 177 images)" dataDxfId="6"/>
-    <tableColumn id="8" name="Classifier training time" dataDxfId="5"/>
-    <tableColumn id="9" name="Classifier test time - 177 images_x000a_(sliding window with 482 ROIs per image)" dataDxfId="4"/>
-    <tableColumn id="10" name="Accuracy" dataDxfId="3"/>
-    <tableColumn id="11" name="Precision" dataDxfId="2"/>
-    <tableColumn id="12" name="Recall" dataDxfId="1"/>
+    <tableColumn id="1" name="Feature_x000a_detector" dataDxfId="11"/>
+    <tableColumn id="2" name="Feature_x000a_descriptor" dataDxfId="10"/>
+    <tableColumn id="3" name="Feature_x000a_matcher" dataDxfId="9"/>
+    <tableColumn id="4" name="Classifier" dataDxfId="8"/>
+    <tableColumn id="5" name="Vocabulary build time_x000a_(1000 word size - 177 images)" dataDxfId="7"/>
+    <tableColumn id="6" name="Training samples build time_x000a_(177 images)" dataDxfId="6"/>
+    <tableColumn id="7" name="Training samples retrieved_x000a_(from 177 images)" dataDxfId="5"/>
+    <tableColumn id="8" name="Classifier training time" dataDxfId="4"/>
+    <tableColumn id="9" name="Classifier test time - 177 images_x000a_(sliding window with 482 ROIs per image)" dataDxfId="3"/>
+    <tableColumn id="10" name="Accuracy" dataDxfId="2"/>
+    <tableColumn id="11" name="Precision" dataDxfId="1"/>
+    <tableColumn id="12" name="Recall" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1421,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,20 +1475,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1574,42 +1604,42 @@
         <v>0.214</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
+      <c r="B5" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="E5" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="16">
         <v>403</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="L5" s="8">
-        <v>0.36199999999999999</v>
+      <c r="H5" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="J5" s="16">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="K5" s="16">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="L5" s="17">
+        <v>0.23400000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1617,7 +1647,7 @@
         <v>102</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -1626,180 +1656,180 @@
         <v>135</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G6" s="2">
         <v>403</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J6" s="2">
-        <v>0.84099999999999997</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="K6" s="2">
-        <v>0.27600000000000002</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="L6" s="8">
-        <v>0.27700000000000002</v>
+        <v>0.36199999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="G7" s="2">
-        <v>447</v>
+        <v>403</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="J7" s="2">
-        <v>0.83899999999999997</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="K7" s="2">
-        <v>0.20599999999999999</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="L7" s="8">
-        <v>0.19500000000000001</v>
+        <v>0.27700000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="G8" s="2">
-        <v>403</v>
+        <v>447</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="J8" s="2">
-        <v>0.81499999999999995</v>
+        <v>0.83899999999999997</v>
       </c>
       <c r="K8" s="2">
-        <v>0.27400000000000002</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="L8" s="8">
-        <v>0.27900000000000003</v>
+        <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="G9" s="2">
-        <v>457</v>
+        <v>403</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="J9" s="2">
         <v>0.81499999999999995</v>
       </c>
       <c r="K9" s="2">
-        <v>0.16800000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="L9" s="8">
-        <v>0.20200000000000001</v>
+        <v>0.27900000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="G10" s="2">
-        <v>488</v>
+        <v>457</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="J10" s="2">
-        <v>0.79400000000000004</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="K10" s="2">
-        <v>0.217</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="L10" s="8">
-        <v>0.29599999999999999</v>
+        <v>0.20200000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1813,31 +1843,31 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G11" s="2">
         <v>488</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>26</v>
+        <v>130</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>27</v>
+        <v>131</v>
       </c>
       <c r="J11" s="2">
-        <v>0.78400000000000003</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="K11" s="2">
-        <v>0.24199999999999999</v>
+        <v>0.217</v>
       </c>
       <c r="L11" s="8">
-        <v>0.38500000000000001</v>
+        <v>0.29599999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1848,42 +1878,42 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G12" s="2">
         <v>488</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="J12" s="2">
-        <v>0.77600000000000002</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="K12" s="2">
-        <v>0.251</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="L12" s="8">
-        <v>0.41099999999999998</v>
+        <v>0.38500000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -1892,36 +1922,36 @@
         <v>135</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G13" s="2">
-        <v>447</v>
+        <v>488</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="J13" s="2">
-        <v>0.73899999999999999</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="K13" s="2">
-        <v>0.23899999999999999</v>
+        <v>0.251</v>
       </c>
       <c r="L13" s="8">
-        <v>0.54900000000000004</v>
+        <v>0.41099999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -1930,28 +1960,28 @@
         <v>135</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G14" s="2">
-        <v>488</v>
+        <v>447</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="J14" s="2">
-        <v>0.71399999999999997</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="K14" s="2">
-        <v>0.219</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="L14" s="8">
-        <v>0.54300000000000004</v>
+        <v>0.54900000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1962,80 +1992,80 @@
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="G15" s="2">
         <v>488</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J15" s="2">
-        <v>0.70499999999999996</v>
+        <v>0.71399999999999997</v>
       </c>
       <c r="K15" s="2">
-        <v>0.21299999999999999</v>
+        <v>0.219</v>
       </c>
       <c r="L15" s="8">
-        <v>0.52800000000000002</v>
+        <v>0.54300000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="G16" s="2">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="J16" s="2">
-        <v>0.69899999999999995</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="K16" s="2">
-        <v>0.20100000000000001</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="L16" s="8">
-        <v>0.47799999999999998</v>
+        <v>0.52800000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
@@ -2044,36 +2074,36 @@
         <v>135</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="G17" s="2">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="J17" s="2">
-        <v>0.67200000000000004</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="K17" s="2">
-        <v>0.24099999999999999</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="L17" s="8">
-        <v>0.73499999999999999</v>
+        <v>0.47799999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
@@ -2082,36 +2112,36 @@
         <v>135</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G18" s="2">
-        <v>514</v>
+        <v>464</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J18" s="2">
-        <v>0.66600000000000004</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="K18" s="2">
-        <v>0.20399999999999999</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="L18" s="8">
-        <v>0.59599999999999997</v>
+        <v>0.73499999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
@@ -2120,36 +2150,36 @@
         <v>135</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="G19" s="2">
-        <v>464</v>
+        <v>514</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="J19" s="2">
-        <v>0.66100000000000003</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="K19" s="2">
-        <v>0.21299999999999999</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="L19" s="8">
-        <v>0.68200000000000005</v>
+        <v>0.59599999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>6</v>
@@ -2158,28 +2188,28 @@
         <v>135</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="G20" s="2">
-        <v>488</v>
+        <v>464</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="J20" s="2">
-        <v>0.61599999999999999</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="K20" s="2">
-        <v>0.187</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="L20" s="8">
-        <v>0.66100000000000003</v>
+        <v>0.68200000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2187,37 +2217,37 @@
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G21" s="2">
         <v>488</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J21" s="2">
-        <v>0.60599999999999998</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="K21" s="2">
-        <v>0.188</v>
+        <v>0.187</v>
       </c>
       <c r="L21" s="8">
-        <v>0.69599999999999995</v>
+        <v>0.66100000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2228,34 +2258,34 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G22" s="2">
         <v>488</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J22" s="2">
-        <v>0.60499999999999998</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="K22" s="2">
-        <v>0.191</v>
+        <v>0.188</v>
       </c>
       <c r="L22" s="8">
-        <v>0.71699999999999997</v>
+        <v>0.69599999999999995</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2263,113 +2293,113 @@
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G23" s="2">
         <v>488</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="J23" s="2">
-        <v>0.60099999999999998</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="K23" s="2">
         <v>0.191</v>
       </c>
       <c r="L23" s="8">
-        <v>0.73199999999999998</v>
+        <v>0.71699999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="G24" s="2">
-        <v>464</v>
+        <v>488</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="J24" s="2">
-        <v>0.57899999999999996</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="K24" s="2">
         <v>0.191</v>
       </c>
       <c r="L24" s="8">
-        <v>0.80100000000000005</v>
+        <v>0.73199999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="G25" s="2">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="J25" s="2">
-        <v>0.57799999999999996</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="K25" s="2">
-        <v>0.17499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="L25" s="8">
-        <v>0.64800000000000002</v>
+        <v>0.80100000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2383,31 +2413,31 @@
         <v>6</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G26" s="2">
         <v>457</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="J26" s="2">
-        <v>0.503</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="K26" s="2">
-        <v>0.17199999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="L26" s="8">
-        <v>0.84699999999999998</v>
+        <v>0.64800000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2421,31 +2451,31 @@
         <v>6</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G27" s="2">
         <v>457</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="J27" s="2">
-        <v>0.499</v>
+        <v>0.503</v>
       </c>
       <c r="K27" s="2">
-        <v>0.17100000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="L27" s="8">
-        <v>0.84499999999999997</v>
+        <v>0.84699999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2459,219 +2489,257 @@
         <v>6</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G28" s="2">
         <v>457</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="J28" s="2">
-        <v>0.46899999999999997</v>
+        <v>0.499</v>
       </c>
       <c r="K28" s="2">
-        <v>0.16700000000000001</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="L28" s="8">
-        <v>0.86399999999999999</v>
+        <v>0.84499999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="G29" s="2">
-        <v>487</v>
+        <v>457</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="J29" s="2">
-        <v>0.44600000000000001</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="K29" s="2">
-        <v>0.16500000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="L29" s="8">
-        <v>0.88600000000000001</v>
+        <v>0.86399999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="2">
+        <v>487</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="L30" s="8">
+        <v>0.88600000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G31" s="2">
         <v>457</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J31" s="2">
         <v>0.42299999999999999</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K31" s="2">
         <v>0.161</v>
       </c>
-      <c r="L30" s="8">
+      <c r="L31" s="8">
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B32" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F32" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G32" s="10">
         <v>488</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H32" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I31" s="10" t="s">
+      <c r="I32" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J32" s="10">
         <v>0.42099999999999999</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K32" s="10">
         <v>0.159</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L32" s="11">
         <v>0.88900000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="4:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D33" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
     </row>
     <row r="34" spans="4:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D34" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+        <v>142</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="4:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D35" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="4:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D36" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E36" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="12" t="s">
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="12" t="s">
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="12" t="s">
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="D37:I37"/>
+    <mergeCell ref="D40:I40"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="D38:I38"/>
-    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="D39:I39"/>
     <mergeCell ref="E34:H34"/>
     <mergeCell ref="E35:H35"/>
-    <mergeCell ref="D39:I39"/>
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="E36:H36"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>